<commit_message>
added base of offset logic
</commit_message>
<xml_diff>
--- a/Modbus_Tags.xlsx
+++ b/Modbus_Tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e0d199abbb6f1b9/Documents/GitHub/Alchemy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD141FE7-5B60-413F-8C8E-24EB51CA6F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{CD141FE7-5B60-413F-8C8E-24EB51CA6F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209846A2-4395-4E04-BB74-08554F37AB22}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
+    <workbookView xWindow="4152" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Tag List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="188">
   <si>
     <t>Data Type</t>
   </si>
@@ -131,21 +131,6 @@
     <t xml:space="preserve">Array Index </t>
   </si>
   <si>
-    <t>Phase Mix</t>
-  </si>
-  <si>
-    <t>Phase Initalize</t>
-  </si>
-  <si>
-    <t>Phase Idle</t>
-  </si>
-  <si>
-    <t>Phase Dispense</t>
-  </si>
-  <si>
-    <t>Phase End</t>
-  </si>
-  <si>
     <t>MB_HR[0]</t>
   </si>
   <si>
@@ -194,15 +179,9 @@
     <t>MB_C[13]</t>
   </si>
   <si>
-    <t>Internal Boolean Data</t>
-  </si>
-  <si>
     <t>011</t>
   </si>
   <si>
-    <t>012</t>
-  </si>
-  <si>
     <t>013</t>
   </si>
   <si>
@@ -596,17 +575,41 @@
     <t>AVG</t>
   </si>
   <si>
-    <t>EndTime</t>
-  </si>
-  <si>
     <t>MB_HR[15]</t>
+  </si>
+  <si>
+    <t>Station#1Offset</t>
+  </si>
+  <si>
+    <t>MB_HR[16]</t>
+  </si>
+  <si>
+    <t>MB_HR[17]</t>
+  </si>
+  <si>
+    <t>MB_HR[18]</t>
+  </si>
+  <si>
+    <t>MB_HR[19]</t>
+  </si>
+  <si>
+    <t>MB_HR[21]</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>1 = 1/10 a sec</t>
+  </si>
+  <si>
+    <t>MB_HR[20]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,7 +647,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,18 +662,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -717,11 +714,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -730,9 +736,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -748,14 +751,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -763,6 +760,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7809,23 +7825,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85483887-8404-42FC-A14C-0D59A783FB69}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8984375" customWidth="1"/>
-    <col min="4" max="4" width="9.09765625" style="3"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="3"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7842,7 +7859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -7856,10 +7873,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -7873,10 +7890,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7890,10 +7907,10 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7907,10 +7924,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -7924,10 +7941,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -7941,13 +7958,11 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>36</v>
+      </c>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -7961,13 +7976,11 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>37</v>
+      </c>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -7981,13 +7994,11 @@
         <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>38</v>
+      </c>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -8001,13 +8012,11 @@
         <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>39</v>
+      </c>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -8021,13 +8030,11 @@
         <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>30</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -8041,15 +8048,13 @@
         <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>40</v>
+      </c>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -8057,27 +8062,40 @@
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>52</v>
+      <c r="D13" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="22"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>44</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -8085,169 +8103,178 @@
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>54</v>
+      <c r="D15" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>45</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>55</v>
+      <c r="D16" s="2">
+        <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="10">
+        <v>48</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>49</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="2">
-        <v>47</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D24" s="2">
+        <v>410</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11">
-        <v>48</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="11">
-        <v>49</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
@@ -8256,15 +8283,15 @@
         <v>3</v>
       </c>
       <c r="D25" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
@@ -8273,15 +8300,15 @@
         <v>3</v>
       </c>
       <c r="D26" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
@@ -8290,66 +8317,66 @@
         <v>3</v>
       </c>
       <c r="D27" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2">
-        <v>413</v>
+      <c r="D28" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>134</v>
+      <c r="D29" s="2">
+        <v>414</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="2">
-        <v>414</v>
+      <c r="D30" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>17</v>
@@ -8357,16 +8384,16 @@
       <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>143</v>
+      <c r="D31" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>17</v>
@@ -8374,16 +8401,16 @@
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>144</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>17</v>
@@ -8391,16 +8418,16 @@
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>151</v>
+      <c r="D33" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
@@ -8408,16 +8435,16 @@
       <c r="C34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>152</v>
+      <c r="D34" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>17</v>
@@ -8425,16 +8452,16 @@
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>153</v>
+      <c r="D35" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>17</v>
@@ -8442,16 +8469,16 @@
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>154</v>
+      <c r="D36" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>17</v>
@@ -8459,50 +8486,50 @@
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>155</v>
+      <c r="D37" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>162</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>156</v>
+      <c r="D38" s="2">
+        <v>415</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="12" t="s">
-        <v>163</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="2">
-        <v>415</v>
+      <c r="D39" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="12" t="s">
-        <v>171</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>17</v>
@@ -8510,16 +8537,16 @@
       <c r="C40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>165</v>
+      <c r="D40" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="12" t="s">
-        <v>172</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>17</v>
@@ -8527,44 +8554,137 @@
       <c r="C41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>166</v>
+      <c r="D41" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="13" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>170</v>
+      <c r="D42" s="2">
+        <v>417</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="13" t="s">
-        <v>185</v>
+        <v>180</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D43" s="2">
-        <v>416</v>
-      </c>
-      <c r="E43" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2">
+        <v>419</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="2">
+        <v>420</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>421</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2">
+        <v>422</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="17" t="s">
         <v>186</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8576,190 +8696,190 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.09765625" customWidth="1"/>
-    <col min="2" max="2" width="26.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.8984375" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="6"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="C16" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -8775,160 +8895,160 @@
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
-      <c r="A1" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15">
+      <c r="B6" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="17"/>
-    </row>
-    <row r="11" spans="1:10" ht="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-    </row>
-    <row r="18" spans="1:2" ht="15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="27" spans="1:2" ht="15">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-    </row>
-    <row r="28" spans="1:2" ht="15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" customFormat="1"/>
-    <row r="34" customFormat="1"/>
-    <row r="35" customFormat="1"/>
-    <row r="36" customFormat="1"/>
-    <row r="37" customFormat="1"/>
-    <row r="38" customFormat="1"/>
-    <row r="39" customFormat="1"/>
-    <row r="40" customFormat="1"/>
-    <row r="41" customFormat="1"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
@@ -8949,490 +9069,490 @@
       <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.3984375" customWidth="1"/>
-    <col min="9" max="9" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.44140625" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.3984375" customWidth="1"/>
+    <col min="16" max="16" width="1.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15">
-      <c r="A1" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="15">
-      <c r="A2" s="6">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>25.04</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>25.1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>25.14</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>26.09</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>25.94</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="13">
         <v>25.96</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="6">
+      <c r="H2" s="12"/>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <f t="shared" ref="J2:K6" si="0">600/(B2/60)</f>
         <v>1437.6996805111821</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <f t="shared" si="0"/>
         <v>1434.2629482071713</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <f t="shared" ref="L2:L6" si="1">600/(D2/60)</f>
         <v>1431.9809069212411</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <f t="shared" ref="M2:M6" si="2">600/(E2/60)</f>
         <v>1379.8390187811422</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <f t="shared" ref="N2:N6" si="3">600/(F2/60)</f>
         <v>1387.8180416345413</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <f>600/(G3/60)</f>
         <v>1410.6583072100314</v>
       </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="6">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="5">
         <f t="shared" ref="Q2:Q6" si="4">AVERAGE(J2:O2)</f>
         <v>1413.7098172108851</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15">
-      <c r="A3" s="6">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>24.65</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>24.94</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>24.92</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>25.19</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>25.99</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>25.52</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="6">
+      <c r="H3" s="12"/>
+      <c r="I3" s="5">
         <v>2</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <f t="shared" si="0"/>
         <v>1460.4462474645031</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <f t="shared" si="0"/>
         <v>1443.4643143544506</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <f t="shared" si="1"/>
         <v>1444.6227929373995</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <f t="shared" si="2"/>
         <v>1429.1385470424771</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <f t="shared" si="3"/>
         <v>1385.148133897653</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <f>600/(G3/60)</f>
         <v>1410.6583072100314</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="6">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="5">
         <f t="shared" si="4"/>
         <v>1428.9130571510859</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15">
-      <c r="A4" s="6">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>24.07</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>24.45</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>25.02</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>26.95</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>25.27</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>24.94</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="6">
+      <c r="H4" s="12"/>
+      <c r="I4" s="5">
         <v>3</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <f t="shared" si="0"/>
         <v>1495.6377233070211</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <f t="shared" si="0"/>
         <v>1472.39263803681</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <f t="shared" si="1"/>
         <v>1438.8489208633093</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <f t="shared" si="2"/>
         <v>1335.8070500927645</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <f t="shared" si="3"/>
         <v>1424.6141669964386</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <f t="shared" ref="O4:O6" si="5">600/(G4/60)</f>
         <v>1443.4643143544506</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="6">
+      <c r="P4" s="12"/>
+      <c r="Q4" s="5">
         <f t="shared" si="4"/>
         <v>1435.127468941799</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15">
-      <c r="A5" s="6">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>24</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>23.6</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>24.54</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>24.9</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>25.49</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>25.33</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="6">
+      <c r="H5" s="12"/>
+      <c r="I5" s="5">
         <v>4</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <f t="shared" si="0"/>
         <v>1525.4237288135591</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <f t="shared" si="1"/>
         <v>1466.9926650366749</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <f t="shared" si="2"/>
         <v>1445.7831325301206</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <f t="shared" si="3"/>
         <v>1412.3185562965871</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <f t="shared" si="5"/>
         <v>1421.2396367943152</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="6">
+      <c r="P5" s="12"/>
+      <c r="Q5" s="5">
         <f t="shared" si="4"/>
         <v>1461.9596199118762</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15">
-      <c r="A6" s="6">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>23</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>23.28</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>24.37</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>24.7</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>24.3</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>24.86</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="6">
+      <c r="H6" s="12"/>
+      <c r="I6" s="5">
         <v>5</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f t="shared" si="0"/>
         <v>1565.2173913043478</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <f t="shared" si="0"/>
         <v>1546.3917525773195</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <f t="shared" si="1"/>
         <v>1477.2260976610587</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <f t="shared" si="2"/>
         <v>1457.48987854251</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <f t="shared" si="3"/>
         <v>1481.4814814814813</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <f t="shared" si="5"/>
         <v>1448.1094127111826</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="6">
+      <c r="P6" s="12"/>
+      <c r="Q6" s="5">
         <f t="shared" si="4"/>
         <v>1495.98600237965</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15">
-      <c r="A7" s="6">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>22.66</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>23.55</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>22.85</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>22.65</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>22.81</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>23</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="6">
+      <c r="H7" s="12"/>
+      <c r="I7" s="5">
         <v>6</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f>600/(B7/60)</f>
         <v>1588.7025595763459</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <f t="shared" ref="K7:O7" si="6">600/(C7/60)</f>
         <v>1528.6624203821655</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <f t="shared" si="6"/>
         <v>1575.4923413566739</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <f t="shared" si="6"/>
         <v>1589.4039735099338</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <f t="shared" si="6"/>
         <v>1578.255151249452</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <f t="shared" si="6"/>
         <v>1565.2173913043478</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="6">
+      <c r="P7" s="12"/>
+      <c r="Q7" s="5">
         <f>AVERAGE(J7:O7)</f>
         <v>1570.9556395631532</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="14" customFormat="1" ht="5.25" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-    </row>
-    <row r="9" spans="1:19" ht="15">
-      <c r="A9" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B9" s="6">
+    <row r="8" spans="1:19" s="11" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="5">
         <f>AVERAGE(B2:B7)</f>
         <v>23.903333333333332</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f t="shared" ref="C9:F9" si="7">AVERAGE(C2:C7)</f>
         <v>24.153333333333336</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="7"/>
         <v>24.473333333333333</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f t="shared" si="7"/>
         <v>25.08</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="7"/>
         <v>24.966666666666665</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f>AVERAGE(G3:G7)</f>
         <v>24.729999999999997</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="J9" s="6">
+      <c r="H9" s="12"/>
+      <c r="I9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J9" s="5">
         <f>AVERAGE(J2:J7)</f>
         <v>1507.9506003605668</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <f t="shared" ref="K9:Q9" si="8">AVERAGE(K2:K7)</f>
         <v>1491.7663003952459</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <f t="shared" si="8"/>
         <v>1472.5272874627262</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <f t="shared" si="8"/>
         <v>1439.5769334164913</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <f t="shared" si="8"/>
         <v>1444.9392552593588</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <f t="shared" si="8"/>
         <v>1449.8912282640597</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="6">
+      <c r="P9" s="12"/>
+      <c r="Q9" s="5">
         <f t="shared" si="8"/>
         <v>1467.7752675264082</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>183</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="13" spans="1:19" ht="15">
+        <v>176</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="Q13">
         <v>30.677</v>
       </c>
@@ -9440,7 +9560,7 @@
         <v>1400.6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="Q14">
         <v>23.82</v>
       </c>
@@ -9448,10 +9568,10 @@
         <v>1408.4</v>
       </c>
       <c r="S14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="Q15">
         <v>24.1</v>
       </c>
@@ -9459,7 +9579,7 @@
         <v>1388.2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="Q16">
         <v>35.51</v>
       </c>
@@ -9467,7 +9587,7 @@
         <v>1315.3</v>
       </c>
     </row>
-    <row r="17" spans="17:18" ht="15">
+    <row r="17" spans="17:18" x14ac:dyDescent="0.3">
       <c r="Q17">
         <v>35.11</v>
       </c>
@@ -9475,7 +9595,7 @@
         <v>1322.1</v>
       </c>
     </row>
-    <row r="18" spans="17:18" ht="15">
+    <row r="18" spans="17:18" x14ac:dyDescent="0.3">
       <c r="Q18">
         <v>24.6</v>
       </c>
@@ -9483,7 +9603,7 @@
         <v>1363.6</v>
       </c>
     </row>
-    <row r="21" spans="17:18" ht="15">
+    <row r="21" spans="17:18" x14ac:dyDescent="0.3">
       <c r="Q21">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Added bottle station offset
</commit_message>
<xml_diff>
--- a/Modbus_Tags.xlsx
+++ b/Modbus_Tags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e0d199abbb6f1b9/Documents/GitHub/Alchemy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunca\Documents\GitHub\Alchemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{CD141FE7-5B60-413F-8C8E-24EB51CA6F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209846A2-4395-4E04-BB74-08554F37AB22}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50CC4C7-E746-4805-AB4C-2E4A5F55BC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4152" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
+    <workbookView xWindow="0" yWindow="5535" windowWidth="19200" windowHeight="15345" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Tag List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="196">
   <si>
     <t>Data Type</t>
   </si>
@@ -599,10 +599,34 @@
     <t>Unused</t>
   </si>
   <si>
-    <t>1 = 1/10 a sec</t>
-  </si>
-  <si>
     <t>MB_HR[20]</t>
+  </si>
+  <si>
+    <t>Station#2Offset</t>
+  </si>
+  <si>
+    <t>Station#3Offset</t>
+  </si>
+  <si>
+    <t>Station#4Offset</t>
+  </si>
+  <si>
+    <t>Station#5Offset</t>
+  </si>
+  <si>
+    <t>Station#6Offset</t>
+  </si>
+  <si>
+    <t>int_16</t>
+  </si>
+  <si>
+    <t>1 = 1/4 a sec</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>ParamterHide</t>
   </si>
 </sst>
 </file>
@@ -727,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -754,31 +778,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7825,24 +7839,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85483887-8404-42FC-A14C-0D59A783FB69}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="3"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7859,7 +7873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -7876,7 +7890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -7893,7 +7907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7910,7 +7924,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7927,7 +7941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -7944,7 +7958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -7960,9 +7974,9 @@
       <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -7978,9 +7992,9 @@
       <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -7996,9 +8010,9 @@
       <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -8014,9 +8028,9 @@
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -8032,9 +8046,9 @@
       <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -8050,9 +8064,9 @@
       <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -8068,14 +8082,13 @@
       <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="J13" s="22"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
@@ -8084,18 +8097,16 @@
         <v>3</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -8104,38 +8115,38 @@
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2">
-        <v>42</v>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>50</v>
@@ -8144,18 +8155,18 @@
         <v>3</v>
       </c>
       <c r="D17" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -8164,15 +8175,18 @@
         <v>3</v>
       </c>
       <c r="D18" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>50</v>
@@ -8181,15 +8195,15 @@
         <v>3</v>
       </c>
       <c r="D19" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>50</v>
@@ -8198,15 +8212,15 @@
         <v>3</v>
       </c>
       <c r="D20" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>50</v>
@@ -8215,32 +8229,32 @@
         <v>3</v>
       </c>
       <c r="D21" s="2">
+        <v>46</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
         <v>47</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="10">
-        <v>48</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>50</v>
@@ -8249,32 +8263,32 @@
         <v>3</v>
       </c>
       <c r="D23" s="10">
+        <v>48</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
         <v>49</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
-        <v>410</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
@@ -8283,15 +8297,15 @@
         <v>3</v>
       </c>
       <c r="D25" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>24</v>
@@ -8300,15 +8314,15 @@
         <v>3</v>
       </c>
       <c r="D26" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
@@ -8317,66 +8331,66 @@
         <v>3</v>
       </c>
       <c r="D27" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>127</v>
+      <c r="D28" s="2">
+        <v>413</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="2">
-        <v>414</v>
+      <c r="D29" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>136</v>
+      <c r="D30" s="2">
+        <v>414</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>17</v>
@@ -8385,15 +8399,15 @@
         <v>3</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>17</v>
@@ -8402,15 +8416,15 @@
         <v>3</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>17</v>
@@ -8419,15 +8433,15 @@
         <v>3</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>17</v>
@@ -8436,15 +8450,15 @@
         <v>3</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>17</v>
@@ -8453,15 +8467,15 @@
         <v>3</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>17</v>
@@ -8470,15 +8484,15 @@
         <v>3</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>17</v>
@@ -8487,49 +8501,49 @@
         <v>3</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="2">
-        <v>415</v>
+      <c r="D38" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="16" t="s">
-        <v>164</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>158</v>
+      <c r="D39" s="2">
+        <v>415</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>17</v>
@@ -8538,15 +8552,15 @@
         <v>3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>167</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>17</v>
@@ -8555,130 +8569,147 @@
         <v>3</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
-        <v>179</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="2">
-        <v>417</v>
+      <c r="D42" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D47" s="2">
+        <v>421</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2">
         <v>422</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F47" s="17" t="s">
-        <v>186</v>
+      <c r="F48" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -8696,17 +8727,17 @@
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
         <v>92</v>
@@ -8719,7 +8750,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>84</v>
       </c>
@@ -8739,7 +8770,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -8755,7 +8786,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
@@ -8771,7 +8802,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>87</v>
       </c>
@@ -8787,7 +8818,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>88</v>
       </c>
@@ -8799,7 +8830,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>89</v>
       </c>
@@ -8811,7 +8842,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>90</v>
       </c>
@@ -8823,7 +8854,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>91</v>
       </c>
@@ -8835,7 +8866,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>111</v>
       </c>
@@ -8843,7 +8874,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>112</v>
       </c>
@@ -8851,31 +8882,31 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>114</v>
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
         <v>115</v>
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>116</v>
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>117</v>
       </c>
@@ -8895,19 +8926,19 @@
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
@@ -8915,7 +8946,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -8923,7 +8954,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -8931,7 +8962,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -8939,7 +8970,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -8947,7 +8978,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -8955,7 +8986,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -8963,13 +8994,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -8977,7 +9008,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0</v>
       </c>
@@ -8985,7 +9016,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -8996,7 +9027,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -9004,7 +9035,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>3</v>
       </c>
@@ -9012,43 +9043,43 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
@@ -9069,17 +9100,17 @@
       <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.44140625" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.42578125" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.44140625" customWidth="1"/>
+    <col min="16" max="16" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>175</v>
       </c>
@@ -9128,7 +9159,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -9184,7 +9215,7 @@
         <v>1413.7098172108851</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -9240,7 +9271,7 @@
         <v>1428.9130571510859</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -9296,7 +9327,7 @@
         <v>1435.127468941799</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -9352,7 +9383,7 @@
         <v>1461.9596199118762</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -9408,7 +9439,7 @@
         <v>1495.98600237965</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -9464,7 +9495,7 @@
         <v>1570.9556395631532</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="11" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="11" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -9483,7 +9514,7 @@
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>177</v>
       </c>
@@ -9545,14 +9576,14 @@
         <v>1467.7752675264082</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>176</v>
       </c>
       <c r="H10" s="11"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q13">
         <v>30.677</v>
       </c>
@@ -9560,7 +9591,7 @@
         <v>1400.6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q14">
         <v>23.82</v>
       </c>
@@ -9571,7 +9602,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q15">
         <v>24.1</v>
       </c>
@@ -9579,7 +9610,7 @@
         <v>1388.2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q16">
         <v>35.51</v>
       </c>
@@ -9587,7 +9618,7 @@
         <v>1315.3</v>
       </c>
     </row>
-    <row r="17" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
       <c r="Q17">
         <v>35.11</v>
       </c>
@@ -9595,7 +9626,7 @@
         <v>1322.1</v>
       </c>
     </row>
-    <row r="18" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="17:18" x14ac:dyDescent="0.25">
       <c r="Q18">
         <v>24.6</v>
       </c>
@@ -9603,7 +9634,7 @@
         <v>1363.6</v>
       </c>
     </row>
-    <row r="21" spans="17:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="17:18" x14ac:dyDescent="0.25">
       <c r="Q21">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
missed loop for setting values in PLC
</commit_message>
<xml_diff>
--- a/Modbus_Tags.xlsx
+++ b/Modbus_Tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dunca\Documents\GitHub\Alchemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50CC4C7-E746-4805-AB4C-2E4A5F55BC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3207A4-EB02-4FE3-A7DE-3B9DAC3158F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5535" windowWidth="19200" windowHeight="15345" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4AD5CBED-8372-44A8-B2C4-3A6BCD43FD21}"/>
   </bookViews>
   <sheets>
     <sheet name="Tag List" sheetId="1" r:id="rId1"/>
@@ -7841,8 +7841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85483887-8404-42FC-A14C-0D59A783FB69}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>